<commit_message>
Week 9: Release 0.1
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/lectures/c8-tables.xlsx
+++ b/y2s1/statistics-ii/lectures/c8-tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CDD332-195F-4A8C-8902-7BB19B2171A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FF2EDB-AA98-4EC7-8B6F-340303B5C666}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3840" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
   </bookViews>
   <sheets>
     <sheet name="C8" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>X</t>
   </si>
@@ -100,6 +101,24 @@
   <si>
     <t>Q5</t>
   </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>4 same values at 30</t>
+  </si>
+  <si>
+    <t>average of ranks 2,3,4,5</t>
+  </si>
+  <si>
+    <t>=(2+3+4+5)/4</t>
+  </si>
+  <si>
+    <t>For 31, since the next "rank" after</t>
+  </si>
+  <si>
+    <t>the averages is 6</t>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -369,11 +388,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -402,6 +432,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,8 +516,8 @@
       <xdr:rowOff>6626</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="700320" cy="182935"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -527,6 +559,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -609,7 +642,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -673,8 +706,8 @@
       <xdr:rowOff>180242</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="144976" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -716,6 +749,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -755,7 +789,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -819,8 +853,8 @@
       <xdr:rowOff>2930</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="149080" cy="182935"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -862,6 +896,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -901,7 +936,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -965,8 +1000,8 @@
       <xdr:rowOff>185658</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="700320" cy="182935"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -1008,6 +1043,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1090,7 +1126,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -1154,8 +1190,8 @@
       <xdr:rowOff>8346</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="191073" cy="182154"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1197,6 +1233,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1236,7 +1273,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1278,6 +1315,641 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:r>
+                <a:rPr lang="en-MY" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑^2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>242520</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180242</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="144976" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B555C464-A5B3-4788-8C98-4330E2625DB4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1685924" y="6737838"/>
+              <a:ext cx="144976" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B555C464-A5B3-4788-8C98-4330E2625DB4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1685924" y="6737838"/>
+              <a:ext cx="144976" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-MY" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑟_𝑥</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>233728</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>2930</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="149080" cy="182935"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{976639CD-E0D4-4865-A176-1B50183E0F1C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2893401" y="6758353"/>
+              <a:ext cx="149080" cy="182935"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑦</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{976639CD-E0D4-4865-A176-1B50183E0F1C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2893401" y="6758353"/>
+              <a:ext cx="149080" cy="182935"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-MY" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑟_𝑦</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>59507</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>185658</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="700320" cy="182935"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4177888D-8601-49B3-8B10-C2DCFBD955F1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3327315" y="6743254"/>
+              <a:ext cx="700320" cy="182935"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-MY" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑑</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-MY" sz="1100" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-MY" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-MY" sz="1100" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-MY" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑦</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4177888D-8601-49B3-8B10-C2DCFBD955F1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3327315" y="6743254"/>
+              <a:ext cx="700320" cy="182935"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-MY" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑=𝑟_𝑥−𝑟_𝑦</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>160618</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>8346</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="191073" cy="182154"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF1CB80C-D274-46CF-833C-D3C2AA7DA63E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4249041" y="6763769"/>
+              <a:ext cx="191073" cy="182154"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-MY" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-MY" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-MY" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="TextBox 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF1CB80C-D274-46CF-833C-D3C2AA7DA63E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4249041" y="6763769"/>
+              <a:ext cx="191073" cy="182154"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-MY" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -1592,10 +2264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A3658A-A553-4F9E-8618-7897D8C87AB2}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,6 +3177,317 @@
         <v>0</v>
       </c>
     </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G47" s="26">
+        <f>SUM(G37:G46)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="12"/>
+      <c r="D49" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="24"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>30</v>
+      </c>
+      <c r="C50" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="D50" s="4">
+        <v>30</v>
+      </c>
+      <c r="E50" s="4">
+        <v>9</v>
+      </c>
+      <c r="F50" s="4">
+        <f>C50-E50</f>
+        <v>-5.5</v>
+      </c>
+      <c r="G50" s="4">
+        <f>F50^2</f>
+        <v>30.25</v>
+      </c>
+      <c r="I50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="3">
+        <v>31</v>
+      </c>
+      <c r="C51" s="3">
+        <v>6</v>
+      </c>
+      <c r="D51" s="3">
+        <v>14</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" ref="F51:F61" si="10">C51-E51</f>
+        <v>5</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" ref="G51:G61" si="11">F51^2</f>
+        <v>25</v>
+      </c>
+      <c r="I51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="3">
+        <v>32</v>
+      </c>
+      <c r="C52" s="3">
+        <v>7</v>
+      </c>
+      <c r="D52" s="3">
+        <v>30</v>
+      </c>
+      <c r="E52" s="3">
+        <v>9</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="I52" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
+        <v>30</v>
+      </c>
+      <c r="C53" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D53" s="3">
+        <v>23</v>
+      </c>
+      <c r="E53" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <f>3.5</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="3">
+        <v>46</v>
+      </c>
+      <c r="C54" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="D54" s="3">
+        <v>32</v>
+      </c>
+      <c r="E54" s="3">
+        <v>11</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.5</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="11"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>30</v>
+      </c>
+      <c r="C55" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D55" s="3">
+        <v>26</v>
+      </c>
+      <c r="E55" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="F55" s="3">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="I55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="3">
+        <v>19</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1</v>
+      </c>
+      <c r="D56" s="3">
+        <v>20</v>
+      </c>
+      <c r="E56" s="3">
+        <v>2</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="3">
+        <v>35</v>
+      </c>
+      <c r="C57" s="3">
+        <v>8</v>
+      </c>
+      <c r="D57" s="3">
+        <v>21</v>
+      </c>
+      <c r="E57" s="3">
+        <v>3</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="G57" s="3">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="3">
+        <v>40</v>
+      </c>
+      <c r="C58" s="3">
+        <v>9</v>
+      </c>
+      <c r="D58" s="3">
+        <v>23</v>
+      </c>
+      <c r="E58" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F58" s="3">
+        <f t="shared" si="10"/>
+        <v>4.5</v>
+      </c>
+      <c r="G58" s="3">
+        <f t="shared" si="11"/>
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="3">
+        <v>46</v>
+      </c>
+      <c r="C59" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="D59" s="3">
+        <v>30</v>
+      </c>
+      <c r="E59" s="3">
+        <v>9</v>
+      </c>
+      <c r="F59" s="3">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="G59" s="3">
+        <f t="shared" si="11"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="3">
+        <v>57</v>
+      </c>
+      <c r="C60" s="3">
+        <v>12</v>
+      </c>
+      <c r="D60" s="3">
+        <v>35</v>
+      </c>
+      <c r="E60" s="3">
+        <v>12</v>
+      </c>
+      <c r="F60" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="3">
+        <v>30</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D61" s="3">
+        <v>26</v>
+      </c>
+      <c r="E61" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="F61" s="3">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="G61" s="3">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="26">
+        <f>SUM(G50:G61)</f>
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
y2s1: Week 10 Release 0.1
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/lectures/c8-tables.xlsx
+++ b/y2s1/statistics-ii/lectures/c8-tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FF2EDB-AA98-4EC7-8B6F-340303B5C666}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10AFB2B-D824-4358-A1BE-2518119AB724}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>X</t>
   </si>
@@ -119,6 +119,24 @@
   <si>
     <t>the averages is 6</t>
   </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>SUMS</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
 </sst>
 </file>
 
@@ -162,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -399,11 +417,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -434,6 +524,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,6 +551,1042 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY"/>
+              <a:t>Data</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-MY" baseline="0"/>
+              <a:t> on relationship between advertising expenditure and total sales value</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-MY"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'C8'!$C$89:$C$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'C8'!$D$89:$D$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8F9-452D-B332-B798272BB65A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1214482575"/>
+        <c:axId val="1321819183"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1214482575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>Advertising</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-MY" baseline="0"/>
+                  <a:t> expenditure</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-MY"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1321819183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1321819183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>Total Sales Voluem</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1214482575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1337,8 +2475,8 @@
       <xdr:rowOff>180242</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="144976" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -1420,7 +2558,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -1485,8 +2623,8 @@
       <xdr:rowOff>2930</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="149080" cy="182935"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -1568,7 +2706,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -1633,8 +2771,8 @@
       <xdr:rowOff>185658</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="700320" cy="182935"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -1759,7 +2897,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -1824,8 +2962,8 @@
       <xdr:rowOff>8346</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="191073" cy="182154"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -1907,7 +3045,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -1964,6 +3102,42 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>588066</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>19878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438979</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>96078</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1F0DA4E-F86E-4C8B-9D1E-EA00A9D905C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2264,10 +3438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A3658A-A553-4F9E-8618-7897D8C87AB2}">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3488,6 +4662,697 @@
         <v>127</v>
       </c>
     </row>
+    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="29"/>
+      <c r="C65" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="C66" s="18">
+        <v>20</v>
+      </c>
+      <c r="D66" s="4">
+        <v>82</v>
+      </c>
+      <c r="E66" s="4">
+        <f>C66*D66</f>
+        <v>1640</v>
+      </c>
+      <c r="F66" s="4">
+        <f>C66^2</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="C67" s="3">
+        <v>16</v>
+      </c>
+      <c r="D67" s="3">
+        <v>70</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" ref="E67:E70" si="12">C67*D67</f>
+        <v>1120</v>
+      </c>
+      <c r="F67" s="3">
+        <f t="shared" ref="F67:F70" si="13">C67^2</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3">
+        <v>24</v>
+      </c>
+      <c r="D68" s="3">
+        <v>90</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="12"/>
+        <v>2160</v>
+      </c>
+      <c r="F68" s="3">
+        <f t="shared" si="13"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3">
+        <v>22</v>
+      </c>
+      <c r="D69" s="3">
+        <v>85</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="12"/>
+        <v>1870</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="13"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3">
+        <v>18</v>
+      </c>
+      <c r="D70" s="3">
+        <v>73</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="12"/>
+        <v>1314</v>
+      </c>
+      <c r="F70" s="3">
+        <f t="shared" si="13"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="3">
+        <f>SUM(C66:C70)</f>
+        <v>100</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" ref="D71:E71" si="14">SUM(D66:D70)</f>
+        <v>400</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="14"/>
+        <v>8104</v>
+      </c>
+      <c r="F71" s="3">
+        <f>SUM(F66:F70)</f>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="29"/>
+      <c r="C74" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="4">
+        <v>5</v>
+      </c>
+      <c r="D75" s="4">
+        <v>190</v>
+      </c>
+      <c r="E75" s="4">
+        <f>C75*D75</f>
+        <v>950</v>
+      </c>
+      <c r="F75" s="4">
+        <f>C75^2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+      <c r="C76" s="3">
+        <v>10</v>
+      </c>
+      <c r="D76" s="3">
+        <v>240</v>
+      </c>
+      <c r="E76" s="3">
+        <f t="shared" ref="E76:E84" si="15">C76*D76</f>
+        <v>2400</v>
+      </c>
+      <c r="F76" s="3">
+        <f t="shared" ref="F76:F84" si="16">C76^2</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="3">
+        <v>15</v>
+      </c>
+      <c r="D77" s="3">
+        <v>250</v>
+      </c>
+      <c r="E77" s="3">
+        <f t="shared" si="15"/>
+        <v>3750</v>
+      </c>
+      <c r="F77" s="3">
+        <f t="shared" si="16"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="C78" s="3">
+        <v>20</v>
+      </c>
+      <c r="D78" s="3">
+        <v>300</v>
+      </c>
+      <c r="E78" s="3">
+        <f t="shared" si="15"/>
+        <v>6000</v>
+      </c>
+      <c r="F78" s="3">
+        <f t="shared" si="16"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+      <c r="C79" s="3">
+        <v>30</v>
+      </c>
+      <c r="D79" s="3">
+        <v>310</v>
+      </c>
+      <c r="E79" s="3">
+        <f t="shared" si="15"/>
+        <v>9300</v>
+      </c>
+      <c r="F79" s="3">
+        <f t="shared" si="16"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+      <c r="C80" s="3">
+        <v>30</v>
+      </c>
+      <c r="D80" s="3">
+        <v>335</v>
+      </c>
+      <c r="E80" s="3">
+        <f t="shared" si="15"/>
+        <v>10050</v>
+      </c>
+      <c r="F80" s="3">
+        <f t="shared" si="16"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="3">
+        <v>30</v>
+      </c>
+      <c r="D81" s="3">
+        <v>300</v>
+      </c>
+      <c r="E81" s="3">
+        <f t="shared" si="15"/>
+        <v>9000</v>
+      </c>
+      <c r="F81" s="3">
+        <f t="shared" si="16"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+      <c r="C82" s="3">
+        <v>50</v>
+      </c>
+      <c r="D82" s="3">
+        <v>300</v>
+      </c>
+      <c r="E82" s="3">
+        <f t="shared" si="15"/>
+        <v>15000</v>
+      </c>
+      <c r="F82" s="3">
+        <f t="shared" si="16"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="3">
+        <v>50</v>
+      </c>
+      <c r="D83" s="3">
+        <v>350</v>
+      </c>
+      <c r="E83" s="3">
+        <f t="shared" si="15"/>
+        <v>17500</v>
+      </c>
+      <c r="F83" s="3">
+        <f t="shared" si="16"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="28"/>
+      <c r="C84" s="28">
+        <v>60</v>
+      </c>
+      <c r="D84" s="28">
+        <v>395</v>
+      </c>
+      <c r="E84" s="28">
+        <f t="shared" si="15"/>
+        <v>23700</v>
+      </c>
+      <c r="F84" s="28">
+        <f t="shared" si="16"/>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" s="31">
+        <f>SUM(C75:C84)</f>
+        <v>300</v>
+      </c>
+      <c r="D85" s="31">
+        <f t="shared" ref="D85:F85" si="17">SUM(D75:D84)</f>
+        <v>2970</v>
+      </c>
+      <c r="E85" s="31">
+        <f t="shared" si="17"/>
+        <v>97650</v>
+      </c>
+      <c r="F85" s="32">
+        <f t="shared" si="17"/>
+        <v>12050</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="29"/>
+      <c r="C88" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E88" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F88" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G88" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="4"/>
+      <c r="C89" s="4">
+        <v>20</v>
+      </c>
+      <c r="D89" s="4">
+        <v>160</v>
+      </c>
+      <c r="E89" s="4">
+        <f>C89*D89</f>
+        <v>3200</v>
+      </c>
+      <c r="F89" s="34">
+        <f>C89^2</f>
+        <v>400</v>
+      </c>
+      <c r="G89" s="4">
+        <f>D89^2</f>
+        <v>25600</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="3"/>
+      <c r="C90" s="3">
+        <v>25</v>
+      </c>
+      <c r="D90" s="3">
+        <v>250</v>
+      </c>
+      <c r="E90" s="3">
+        <f t="shared" ref="E90:E96" si="18">C90*D90</f>
+        <v>6250</v>
+      </c>
+      <c r="F90" s="35">
+        <f t="shared" ref="F90:F96" si="19">C90^2</f>
+        <v>625</v>
+      </c>
+      <c r="G90" s="3">
+        <f t="shared" ref="G90:G96" si="20">D90^2</f>
+        <v>62500</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3">
+        <v>40</v>
+      </c>
+      <c r="D91" s="3">
+        <v>420</v>
+      </c>
+      <c r="E91" s="3">
+        <f t="shared" si="18"/>
+        <v>16800</v>
+      </c>
+      <c r="F91" s="35">
+        <f t="shared" si="19"/>
+        <v>1600</v>
+      </c>
+      <c r="G91" s="3">
+        <f t="shared" si="20"/>
+        <v>176400</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="3"/>
+      <c r="C92" s="3">
+        <v>10</v>
+      </c>
+      <c r="D92" s="3">
+        <v>80</v>
+      </c>
+      <c r="E92" s="3">
+        <f t="shared" si="18"/>
+        <v>800</v>
+      </c>
+      <c r="F92" s="35">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+      <c r="G92" s="3">
+        <f t="shared" si="20"/>
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="3"/>
+      <c r="C93" s="3">
+        <v>60</v>
+      </c>
+      <c r="D93" s="3">
+        <v>900</v>
+      </c>
+      <c r="E93" s="3">
+        <f t="shared" si="18"/>
+        <v>54000</v>
+      </c>
+      <c r="F93" s="35">
+        <f t="shared" si="19"/>
+        <v>3600</v>
+      </c>
+      <c r="G93" s="3">
+        <f t="shared" si="20"/>
+        <v>810000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="3"/>
+      <c r="C94" s="3">
+        <v>35</v>
+      </c>
+      <c r="D94" s="3">
+        <v>360</v>
+      </c>
+      <c r="E94" s="3">
+        <f t="shared" si="18"/>
+        <v>12600</v>
+      </c>
+      <c r="F94" s="35">
+        <f t="shared" si="19"/>
+        <v>1225</v>
+      </c>
+      <c r="G94" s="3">
+        <f t="shared" si="20"/>
+        <v>129600</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="3"/>
+      <c r="C95" s="3">
+        <v>55</v>
+      </c>
+      <c r="D95" s="3">
+        <v>700</v>
+      </c>
+      <c r="E95" s="3">
+        <f t="shared" si="18"/>
+        <v>38500</v>
+      </c>
+      <c r="F95" s="35">
+        <f t="shared" si="19"/>
+        <v>3025</v>
+      </c>
+      <c r="G95" s="3">
+        <f t="shared" si="20"/>
+        <v>490000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="28"/>
+      <c r="C96" s="28">
+        <v>45</v>
+      </c>
+      <c r="D96" s="28">
+        <v>500</v>
+      </c>
+      <c r="E96" s="28">
+        <f t="shared" si="18"/>
+        <v>22500</v>
+      </c>
+      <c r="F96" s="36">
+        <f t="shared" si="19"/>
+        <v>2025</v>
+      </c>
+      <c r="G96" s="28">
+        <f t="shared" si="20"/>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" s="31">
+        <f>SUM(C89:C96)</f>
+        <v>290</v>
+      </c>
+      <c r="D97" s="31">
+        <f>SUM(D89:D96)</f>
+        <v>3370</v>
+      </c>
+      <c r="E97" s="31">
+        <f>SUM(E89:E96)</f>
+        <v>154650</v>
+      </c>
+      <c r="F97" s="33">
+        <f>SUM(F89:F96)</f>
+        <v>12600</v>
+      </c>
+      <c r="G97" s="19">
+        <f>SUM(G89:G96)</f>
+        <v>1950500</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C116" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E116" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F116" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="17">
+        <v>1998</v>
+      </c>
+      <c r="C117" s="18">
+        <v>0</v>
+      </c>
+      <c r="D117" s="4">
+        <v>103</v>
+      </c>
+      <c r="E117" s="4">
+        <f>C117*D117</f>
+        <v>0</v>
+      </c>
+      <c r="F117" s="4">
+        <f>C117^2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="39">
+        <v>1999</v>
+      </c>
+      <c r="C118" s="2">
+        <v>1</v>
+      </c>
+      <c r="D118" s="3">
+        <v>167</v>
+      </c>
+      <c r="E118" s="3">
+        <f t="shared" ref="E118:E121" si="21">C118*D118</f>
+        <v>167</v>
+      </c>
+      <c r="F118" s="3">
+        <f t="shared" ref="F118:F121" si="22">C118^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B119" s="39">
+        <v>2000</v>
+      </c>
+      <c r="C119" s="2">
+        <v>2</v>
+      </c>
+      <c r="D119" s="3">
+        <v>214</v>
+      </c>
+      <c r="E119" s="3">
+        <f t="shared" si="21"/>
+        <v>428</v>
+      </c>
+      <c r="F119" s="3">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B120" s="39">
+        <v>2001</v>
+      </c>
+      <c r="C120" s="2">
+        <v>3</v>
+      </c>
+      <c r="D120" s="3">
+        <v>262</v>
+      </c>
+      <c r="E120" s="3">
+        <f t="shared" si="21"/>
+        <v>786</v>
+      </c>
+      <c r="F120" s="3">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="21">
+        <v>2002</v>
+      </c>
+      <c r="C121" s="38">
+        <v>4</v>
+      </c>
+      <c r="D121" s="28">
+        <v>309</v>
+      </c>
+      <c r="E121" s="28">
+        <f t="shared" si="21"/>
+        <v>1236</v>
+      </c>
+      <c r="F121" s="28">
+        <f t="shared" si="22"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C122" s="30">
+        <f>SUM(C117:C121)</f>
+        <v>10</v>
+      </c>
+      <c r="D122" s="31">
+        <f>SUM(D117:D121)</f>
+        <v>1055</v>
+      </c>
+      <c r="E122" s="31">
+        <f t="shared" ref="E122:F122" si="23">SUM(E117:E121)</f>
+        <v>2617</v>
+      </c>
+      <c r="F122" s="32">
+        <f t="shared" si="23"/>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
y2s1: Week 12 Update 0.1
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/lectures/c8-tables.xlsx
+++ b/y2s1/statistics-ii/lectures/c8-tables.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10AFB2B-D824-4358-A1BE-2518119AB724}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC43B29-C3AF-4144-A9C1-D7AB09406D29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
   </bookViews>
   <sheets>
     <sheet name="C8" sheetId="1" r:id="rId1"/>
+    <sheet name="T8" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
   <si>
     <t>X</t>
   </si>
@@ -136,6 +137,69 @@
   </si>
   <si>
     <t>YEAR</t>
+  </si>
+  <si>
+    <t>Monthly Premium ( RM )</t>
+  </si>
+  <si>
+    <t>Driving Experience ( years )</t>
+  </si>
+  <si>
+    <t>Question 3</t>
+  </si>
+  <si>
+    <t>Difference ^2</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Panel II</t>
+  </si>
+  <si>
+    <t>Panel I</t>
+  </si>
+  <si>
+    <t>Candidate</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Ranking (Purchase Manager)</t>
+  </si>
+  <si>
+    <t>Ranking (Store Manager)</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Purchase Manager</t>
+  </si>
+  <si>
+    <t>Store Manager</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Weeks of experience ( X )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of rejects ( Y ) </t>
+  </si>
+  <si>
+    <t>PMCC:</t>
+  </si>
+  <si>
+    <t>SRCC:</t>
   </si>
 </sst>
 </file>
@@ -1033,6 +1097,978 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'T8'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monthly Premium ( RM )</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'T8'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'T8'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-95B2-4B8A-BEE9-ACE4F666D317}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="812028111"/>
+        <c:axId val="812110175"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="812028111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>Driving Experience ( years )</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812110175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="812110175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>Monthly Premium ( RM )</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="812028111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY"/>
+              <a:t>Scatter plot on the</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-MY" baseline="0"/>
+              <a:t> relationship between weeks of experience and number of rejects</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-MY"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'T8'!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of rejects ( Y ) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'T8'!$B$43:$I$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'T8'!$B$44:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC80-4FDB-84E8-B0E9A3ABBE9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1876755376"/>
+        <c:axId val="1876920112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1876755376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>Weeks of experience</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1876920112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1876920112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>Number of rejects</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1876755376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1073,7 +2109,1105 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3141,6 +5275,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B2D008-1375-4B9F-BF29-DB5E4194EB6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50348</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>355148</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>134030</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DD78491-AE58-44F2-ADA9-87CBF7DFA0E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3440,7 +5651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A3658A-A553-4F9E-8618-7897D8C87AB2}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A125" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
@@ -5358,4 +7569,652 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725D82E5-2E75-4392-B55B-81B45DEC23B3}">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <v>9</v>
+      </c>
+      <c r="F1">
+        <v>15</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>25</v>
+      </c>
+      <c r="I1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>64</v>
+      </c>
+      <c r="C2">
+        <v>87</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>71</v>
+      </c>
+      <c r="F2">
+        <v>44</v>
+      </c>
+      <c r="G2">
+        <v>56</v>
+      </c>
+      <c r="H2">
+        <v>42</v>
+      </c>
+      <c r="I2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <f>B28-B29</f>
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f>C28-C29</f>
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <f>D28-D29</f>
+        <v>-3</v>
+      </c>
+      <c r="E30">
+        <f>E28-E29</f>
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <f>F28-F29</f>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>G28-G29</f>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f>H28-H29</f>
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f>I28-I29</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <f>B30^2</f>
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f>C30^2</f>
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <f>D30^2</f>
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <f>E30^2</f>
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <f>F30^2</f>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f>G30^2</f>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f>H30^2</f>
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <f>I30^2</f>
+        <v>9</v>
+      </c>
+      <c r="J31" s="1">
+        <f>SUM(B31:I31)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="H36">
+        <v>9</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36">
+        <v>10</v>
+      </c>
+      <c r="K36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>6</v>
+      </c>
+      <c r="I37">
+        <v>7</v>
+      </c>
+      <c r="J37">
+        <v>8</v>
+      </c>
+      <c r="K37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <f>B36-B37</f>
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <f>C36-C37</f>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f>D36-D37</f>
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <f>E36-E37</f>
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f>F36-F37</f>
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <f>G36-G37</f>
+        <v>-3</v>
+      </c>
+      <c r="H38">
+        <f>H36-H37</f>
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <f>I36-I37</f>
+        <v>-4</v>
+      </c>
+      <c r="J38">
+        <f>J36-J37</f>
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <f>K36-K37</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f>B38^2</f>
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <f>C38^2</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>D38^2</f>
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <f>E38^2</f>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f>F38^2</f>
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <f>G38^2</f>
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <f>H38^2</f>
+        <v>9</v>
+      </c>
+      <c r="I39">
+        <f>I38^2</f>
+        <v>16</v>
+      </c>
+      <c r="J39">
+        <f>J38^2</f>
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <f>K38^2</f>
+        <v>4</v>
+      </c>
+      <c r="L39" s="1">
+        <f>SUM(B39:K39)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>9</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>12</v>
+      </c>
+      <c r="I43">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>22</v>
+      </c>
+      <c r="D44">
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <v>18</v>
+      </c>
+      <c r="F44">
+        <v>14</v>
+      </c>
+      <c r="G44">
+        <v>14</v>
+      </c>
+      <c r="H44">
+        <v>11</v>
+      </c>
+      <c r="I44">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49">
+        <f>PEARSON(B43:I43,B44:I44)</f>
+        <v>-0.87141809054905162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
y2s1: Week 13 Release 0.1
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/lectures/c8-tables.xlsx
+++ b/y2s1/statistics-ii/lectures/c8-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC43B29-C3AF-4144-A9C1-D7AB09406D29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DDC357-7ED5-42B8-8269-E53F956A1CF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
+    <workbookView xWindow="-1155" yWindow="795" windowWidth="15375" windowHeight="7815" activeTab="1" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
   </bookViews>
   <sheets>
     <sheet name="C8" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="69">
   <si>
     <t>X</t>
   </si>
@@ -200,6 +200,45 @@
   </si>
   <si>
     <t>SRCC:</t>
+  </si>
+  <si>
+    <t>Rank X</t>
+  </si>
+  <si>
+    <t>Rank Y</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Question 4</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Output (X)</t>
+  </si>
+  <si>
+    <t>Cost (Y)</t>
+  </si>
+  <si>
+    <t>Question 5</t>
+  </si>
+  <si>
+    <t>Median income ($) (X)</t>
+  </si>
+  <si>
+    <t>House purchase power ($000) (Y)</t>
+  </si>
+  <si>
+    <t>Question 6</t>
+  </si>
+  <si>
+    <t>Year (Let first year be 0) (X)</t>
+  </si>
+  <si>
+    <t>Time (Y)</t>
   </si>
 </sst>
 </file>
@@ -2069,6 +2108,364 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'T8'!$C$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cost (Y)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'T8'!$B$78:$B$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'T8'!$C$78:$C$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6C39-4375-90B5-D08A2818F3A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="807168335"/>
+        <c:axId val="806069023"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="807168335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="806069023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="806069023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="807168335"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2189,6 +2586,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3208,6 +3645,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5349,6 +6302,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>77560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>153760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81B633CA-C8A7-47E3-B08C-E0610AD2EDA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7573,13 +8562,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725D82E5-2E75-4392-B55B-81B45DEC23B3}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M104" sqref="M104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7829,35 +8822,35 @@
         <v>39</v>
       </c>
       <c r="B30">
-        <f>B28-B29</f>
+        <f t="shared" ref="B30:I30" si="0">B28-B29</f>
         <v>1</v>
       </c>
       <c r="C30">
-        <f>C28-C29</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D30">
-        <f>D28-D29</f>
+        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
       <c r="E30">
-        <f>E28-E29</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F30">
-        <f>F28-F29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G30">
-        <f>G28-G29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H30">
-        <f>H28-H29</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I30">
-        <f>I28-I29</f>
+        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
     </row>
@@ -7866,35 +8859,35 @@
         <v>38</v>
       </c>
       <c r="B31">
-        <f>B30^2</f>
+        <f t="shared" ref="B31:I31" si="1">B30^2</f>
         <v>1</v>
       </c>
       <c r="C31">
-        <f>C30^2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D31">
-        <f>D30^2</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E31">
-        <f>E30^2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F31">
-        <f>F30^2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G31">
-        <f>G30^2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H31">
-        <f>H30^2</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I31">
-        <f>I30^2</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J31" s="1">
@@ -8017,43 +9010,43 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <f>B36-B37</f>
+        <f t="shared" ref="B38:K38" si="2">B36-B37</f>
         <v>1</v>
       </c>
       <c r="C38">
-        <f>C36-C37</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D38">
-        <f>D36-D37</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E38">
-        <f>E36-E37</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F38">
-        <f>F36-F37</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G38">
-        <f>G36-G37</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="H38">
-        <f>H36-H37</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I38">
-        <f>I36-I37</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="J38">
-        <f>J36-J37</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K38">
-        <f>K36-K37</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
     </row>
@@ -8062,43 +9055,43 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <f>B38^2</f>
+        <f t="shared" ref="B39:K39" si="3">B38^2</f>
         <v>1</v>
       </c>
       <c r="C39">
-        <f>C38^2</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D39">
-        <f>D38^2</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E39">
-        <f>E38^2</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F39">
-        <f>F38^2</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G39">
-        <f>G38^2</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H39">
-        <f>H38^2</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I39">
-        <f>I38^2</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="J39">
-        <f>J38^2</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="K39">
-        <f>K38^2</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L39" s="1">
@@ -8210,6 +9203,1419 @@
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <v>21</v>
+      </c>
+      <c r="D66">
+        <f>B66*C66</f>
+        <v>84</v>
+      </c>
+      <c r="E66">
+        <f>B66^2</f>
+        <v>16</v>
+      </c>
+      <c r="F66">
+        <f>C66^2</f>
+        <v>441</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>7</v>
+      </c>
+      <c r="I66">
+        <f>G66-H66</f>
+        <v>-6</v>
+      </c>
+      <c r="J66">
+        <f>I66^2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>22</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D73" si="4">B67*C67</f>
+        <v>110</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E73" si="5">B67^2</f>
+        <v>25</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F73" si="6">C67^2</f>
+        <v>484</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>8</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I73" si="7">G67-H67</f>
+        <v>-6</v>
+      </c>
+      <c r="J67">
+        <f t="shared" ref="J67:J73" si="8">I67^2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="6"/>
+        <v>225</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>5</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69">
+        <v>9</v>
+      </c>
+      <c r="C69">
+        <v>18</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="6"/>
+        <v>324</v>
+      </c>
+      <c r="G69">
+        <v>4</v>
+      </c>
+      <c r="H69">
+        <v>6</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70">
+        <v>10</v>
+      </c>
+      <c r="C70">
+        <v>14</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="6"/>
+        <v>196</v>
+      </c>
+      <c r="G70">
+        <v>5</v>
+      </c>
+      <c r="H70">
+        <v>3.5</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="8"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71">
+        <v>11</v>
+      </c>
+      <c r="C71">
+        <v>14</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="5"/>
+        <v>121</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="6"/>
+        <v>196</v>
+      </c>
+      <c r="G71">
+        <v>6</v>
+      </c>
+      <c r="H71">
+        <v>3.5</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="8"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72">
+        <v>12</v>
+      </c>
+      <c r="C72">
+        <v>11</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="6"/>
+        <v>121</v>
+      </c>
+      <c r="G72">
+        <v>7</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>13</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="4"/>
+        <v>182</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="6"/>
+        <v>169</v>
+      </c>
+      <c r="G73">
+        <v>8</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="1">
+        <f>SUM(B66:B73)</f>
+        <v>72</v>
+      </c>
+      <c r="C74" s="1">
+        <f>SUM(C66:C73)</f>
+        <v>128</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" ref="D74:F74" si="9">SUM(D66:D73)</f>
+        <v>1069</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="9"/>
+        <v>732</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="9"/>
+        <v>2156</v>
+      </c>
+      <c r="J74">
+        <f>SUM(J66:J73)</f>
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>20</v>
+      </c>
+      <c r="C78">
+        <v>60</v>
+      </c>
+      <c r="D78">
+        <f>B78*C78</f>
+        <v>1200</v>
+      </c>
+      <c r="E78">
+        <f>B78^2</f>
+        <v>400</v>
+      </c>
+      <c r="F78">
+        <f>C78^2</f>
+        <v>3600</v>
+      </c>
+      <c r="G78">
+        <v>9</v>
+      </c>
+      <c r="H78">
+        <v>9</v>
+      </c>
+      <c r="I78">
+        <f>G78-H78</f>
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <f>I78^2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79">
+        <v>25</v>
+      </c>
+      <c r="D79">
+        <f t="shared" ref="D79:D87" si="10">B79*C79</f>
+        <v>50</v>
+      </c>
+      <c r="E79">
+        <f t="shared" ref="E79:E87" si="11">B79^2</f>
+        <v>4</v>
+      </c>
+      <c r="F79">
+        <f t="shared" ref="F79:F87" si="12">C79^2</f>
+        <v>625</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>2</v>
+      </c>
+      <c r="I79">
+        <f t="shared" ref="I79:I87" si="13">G79-H79</f>
+        <v>-1</v>
+      </c>
+      <c r="J79">
+        <f t="shared" ref="J79:J87" si="14">I79^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <v>26</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="10"/>
+        <v>104</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="12"/>
+        <v>676</v>
+      </c>
+      <c r="G80">
+        <v>2</v>
+      </c>
+      <c r="H80">
+        <v>3</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>4</v>
+      </c>
+      <c r="B81">
+        <v>23</v>
+      </c>
+      <c r="C81">
+        <v>66</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="10"/>
+        <v>1518</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="11"/>
+        <v>529</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="12"/>
+        <v>4356</v>
+      </c>
+      <c r="G81">
+        <v>10</v>
+      </c>
+      <c r="H81">
+        <v>10</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>18</v>
+      </c>
+      <c r="C82">
+        <v>49</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="10"/>
+        <v>882</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="11"/>
+        <v>324</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="12"/>
+        <v>2401</v>
+      </c>
+      <c r="G82">
+        <v>8</v>
+      </c>
+      <c r="H82">
+        <v>8</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>6</v>
+      </c>
+      <c r="B83">
+        <v>14</v>
+      </c>
+      <c r="C83">
+        <v>48</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="10"/>
+        <v>672</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="11"/>
+        <v>196</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="12"/>
+        <v>2304</v>
+      </c>
+      <c r="G83">
+        <v>7</v>
+      </c>
+      <c r="H83">
+        <v>7</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>7</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>35</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="10"/>
+        <v>350</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="12"/>
+        <v>1225</v>
+      </c>
+      <c r="G84">
+        <v>5</v>
+      </c>
+      <c r="H84">
+        <v>5</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>8</v>
+      </c>
+      <c r="B85">
+        <v>8</v>
+      </c>
+      <c r="C85">
+        <v>18</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="10"/>
+        <v>144</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="12"/>
+        <v>324</v>
+      </c>
+      <c r="G85">
+        <v>3.5</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="13"/>
+        <v>2.5</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="14"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>9</v>
+      </c>
+      <c r="B86">
+        <v>13</v>
+      </c>
+      <c r="C86">
+        <v>40</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="10"/>
+        <v>520</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="11"/>
+        <v>169</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="12"/>
+        <v>1600</v>
+      </c>
+      <c r="G86">
+        <v>6</v>
+      </c>
+      <c r="H86">
+        <v>6</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>10</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+      <c r="C87">
+        <v>33</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="10"/>
+        <v>264</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="12"/>
+        <v>1089</v>
+      </c>
+      <c r="G87">
+        <v>3.5</v>
+      </c>
+      <c r="H87">
+        <v>4</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="13"/>
+        <v>-0.5</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="14"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" s="1">
+        <f>SUM(B78:B87)</f>
+        <v>120</v>
+      </c>
+      <c r="C88" s="1">
+        <f t="shared" ref="C88:F88" si="15">SUM(C78:C87)</f>
+        <v>400</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="15"/>
+        <v>5704</v>
+      </c>
+      <c r="E88" s="1">
+        <f t="shared" si="15"/>
+        <v>1866</v>
+      </c>
+      <c r="F88" s="1">
+        <f t="shared" si="15"/>
+        <v>18200</v>
+      </c>
+      <c r="J88">
+        <f>SUM(J78:J87)</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>64</v>
+      </c>
+      <c r="B92">
+        <v>57</v>
+      </c>
+      <c r="C92">
+        <v>54</v>
+      </c>
+      <c r="D92">
+        <v>54</v>
+      </c>
+      <c r="E92">
+        <v>51</v>
+      </c>
+      <c r="F92">
+        <v>63</v>
+      </c>
+      <c r="G92">
+        <v>56</v>
+      </c>
+      <c r="H92">
+        <v>52</v>
+      </c>
+      <c r="I92">
+        <v>56</v>
+      </c>
+      <c r="J92">
+        <v>55</v>
+      </c>
+      <c r="K92">
+        <v>55</v>
+      </c>
+      <c r="L92">
+        <v>56</v>
+      </c>
+      <c r="M92">
+        <v>50</v>
+      </c>
+      <c r="N92" s="1">
+        <f>SUM(B92:M92)</f>
+        <v>659</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>65</v>
+      </c>
+      <c r="B93">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>9</v>
+      </c>
+      <c r="D93">
+        <v>10</v>
+      </c>
+      <c r="E93">
+        <v>12</v>
+      </c>
+      <c r="F93">
+        <v>15</v>
+      </c>
+      <c r="G93">
+        <v>15</v>
+      </c>
+      <c r="H93">
+        <v>12</v>
+      </c>
+      <c r="I93">
+        <v>11</v>
+      </c>
+      <c r="J93">
+        <v>10</v>
+      </c>
+      <c r="K93">
+        <v>10</v>
+      </c>
+      <c r="L93">
+        <v>11</v>
+      </c>
+      <c r="M93">
+        <v>10</v>
+      </c>
+      <c r="N93" s="1">
+        <f>SUM(B93:M93)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <f>B92*B93</f>
+        <v>570</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:M94" si="16">C92*C93</f>
+        <v>486</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="16"/>
+        <v>540</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="16"/>
+        <v>612</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="16"/>
+        <v>945</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="16"/>
+        <v>840</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="16"/>
+        <v>624</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="16"/>
+        <v>616</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="16"/>
+        <v>550</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="16"/>
+        <v>550</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="16"/>
+        <v>616</v>
+      </c>
+      <c r="M94">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="N94" s="1">
+        <f t="shared" ref="N93:N96" si="17">SUM(B94:M94)</f>
+        <v>7449</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <f>B92^2</f>
+        <v>3249</v>
+      </c>
+      <c r="C95">
+        <f t="shared" ref="C95:M95" si="18">C92^2</f>
+        <v>2916</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="18"/>
+        <v>2916</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="18"/>
+        <v>2601</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="18"/>
+        <v>3969</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="18"/>
+        <v>3136</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="18"/>
+        <v>2704</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="18"/>
+        <v>3136</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="18"/>
+        <v>3025</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="18"/>
+        <v>3025</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="18"/>
+        <v>3136</v>
+      </c>
+      <c r="M95">
+        <f t="shared" si="18"/>
+        <v>2500</v>
+      </c>
+      <c r="N95" s="1">
+        <f t="shared" si="17"/>
+        <v>36313</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96">
+        <f>B93^2</f>
+        <v>100</v>
+      </c>
+      <c r="C96">
+        <f t="shared" ref="C96:M96" si="19">C93^2</f>
+        <v>81</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="19"/>
+        <v>144</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="19"/>
+        <v>225</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="19"/>
+        <v>225</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="19"/>
+        <v>144</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="19"/>
+        <v>121</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="19"/>
+        <v>121</v>
+      </c>
+      <c r="M96">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+      <c r="N96" s="1">
+        <f t="shared" si="17"/>
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>56</v>
+      </c>
+      <c r="B97">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>4.5</v>
+      </c>
+      <c r="D97">
+        <v>4.5</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <v>12</v>
+      </c>
+      <c r="G97">
+        <v>9</v>
+      </c>
+      <c r="H97">
+        <v>3</v>
+      </c>
+      <c r="I97">
+        <v>9</v>
+      </c>
+      <c r="J97">
+        <v>6.5</v>
+      </c>
+      <c r="K97">
+        <v>6.5</v>
+      </c>
+      <c r="L97">
+        <v>9</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>57</v>
+      </c>
+      <c r="B98">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>4</v>
+      </c>
+      <c r="E98">
+        <v>9.5</v>
+      </c>
+      <c r="F98">
+        <v>11.5</v>
+      </c>
+      <c r="G98">
+        <v>11.5</v>
+      </c>
+      <c r="H98">
+        <v>9.5</v>
+      </c>
+      <c r="I98">
+        <v>7.5</v>
+      </c>
+      <c r="J98">
+        <v>4</v>
+      </c>
+      <c r="K98">
+        <v>4</v>
+      </c>
+      <c r="L98">
+        <v>7.5</v>
+      </c>
+      <c r="M98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99">
+        <f>(B97-B98)^2</f>
+        <v>49</v>
+      </c>
+      <c r="C99">
+        <f t="shared" ref="C99:M99" si="20">(C97-C98)^2</f>
+        <v>12.25</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="20"/>
+        <v>0.25</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="20"/>
+        <v>56.25</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="20"/>
+        <v>0.25</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="20"/>
+        <v>6.25</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="20"/>
+        <v>42.25</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="20"/>
+        <v>2.25</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="20"/>
+        <v>6.25</v>
+      </c>
+      <c r="K99">
+        <f t="shared" si="20"/>
+        <v>6.25</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="20"/>
+        <v>2.25</v>
+      </c>
+      <c r="M99">
+        <f t="shared" si="20"/>
+        <v>9</v>
+      </c>
+      <c r="N99">
+        <f>SUM(B99:M99)</f>
+        <v>192.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>4</v>
+      </c>
+      <c r="D102">
+        <v>8</v>
+      </c>
+      <c r="E102">
+        <v>12</v>
+      </c>
+      <c r="F102">
+        <v>16</v>
+      </c>
+      <c r="G102">
+        <v>20</v>
+      </c>
+      <c r="H102">
+        <v>24</v>
+      </c>
+      <c r="I102">
+        <v>28</v>
+      </c>
+      <c r="J102">
+        <v>32</v>
+      </c>
+      <c r="K102" s="1">
+        <f>SUM(B102:J102)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B103">
+        <v>58.6</v>
+      </c>
+      <c r="C103">
+        <v>55.7</v>
+      </c>
+      <c r="D103">
+        <v>54.8</v>
+      </c>
+      <c r="E103">
+        <v>55.9</v>
+      </c>
+      <c r="F103">
+        <v>54.9</v>
+      </c>
+      <c r="G103">
+        <v>54.6</v>
+      </c>
+      <c r="H103">
+        <v>54.5</v>
+      </c>
+      <c r="I103">
+        <v>53.8</v>
+      </c>
+      <c r="J103">
+        <v>53.8</v>
+      </c>
+      <c r="K103" s="1">
+        <f t="shared" ref="K103:K106" si="21">SUM(B103:J103)</f>
+        <v>496.60000000000008</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104">
+        <f>B102*B103</f>
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <f t="shared" ref="C104:J104" si="22">C102*C103</f>
+        <v>222.8</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="22"/>
+        <v>438.4</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="22"/>
+        <v>670.8</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="22"/>
+        <v>878.4</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="22"/>
+        <v>1092</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="22"/>
+        <v>1308</v>
+      </c>
+      <c r="I104">
+        <f t="shared" si="22"/>
+        <v>1506.3999999999999</v>
+      </c>
+      <c r="J104">
+        <f t="shared" si="22"/>
+        <v>1721.6</v>
+      </c>
+      <c r="K104" s="1">
+        <f t="shared" si="21"/>
+        <v>7838.4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105">
+        <f>B102^2</f>
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <f t="shared" ref="C105:J105" si="23">C102^2</f>
+        <v>16</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="23"/>
+        <v>64</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="23"/>
+        <v>144</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="23"/>
+        <v>256</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="23"/>
+        <v>400</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="23"/>
+        <v>576</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="23"/>
+        <v>784</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="23"/>
+        <v>1024</v>
+      </c>
+      <c r="K105" s="1">
+        <f t="shared" si="21"/>
+        <v>3264</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <f>B103^2</f>
+        <v>3433.96</v>
+      </c>
+      <c r="C106">
+        <f t="shared" ref="C106:J106" si="24">C103^2</f>
+        <v>3102.4900000000002</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="24"/>
+        <v>3003.0399999999995</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="24"/>
+        <v>3124.81</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="24"/>
+        <v>3014.0099999999998</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="24"/>
+        <v>2981.1600000000003</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="24"/>
+        <v>2970.25</v>
+      </c>
+      <c r="I106">
+        <f t="shared" si="24"/>
+        <v>2894.4399999999996</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="24"/>
+        <v>2894.4399999999996</v>
+      </c>
+      <c r="K106" s="1">
+        <f t="shared" si="21"/>
+        <v>27418.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 13: release 0.2
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/lectures/c8-tables.xlsx
+++ b/y2s1/statistics-ii/lectures/c8-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DDC357-7ED5-42B8-8269-E53F956A1CF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC65F8BB-699D-4E23-A93F-CCB0DF351F89}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1155" yWindow="795" windowWidth="15375" windowHeight="7815" activeTab="1" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
+    <workbookView xWindow="4290" yWindow="1185" windowWidth="15375" windowHeight="7815" activeTab="1" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
   </bookViews>
   <sheets>
     <sheet name="C8" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="76">
   <si>
     <t>X</t>
   </si>
@@ -239,6 +239,27 @@
   </si>
   <si>
     <t>Time (Y)</t>
+  </si>
+  <si>
+    <t>Question 7</t>
+  </si>
+  <si>
+    <t>Average annual earnings ($ '000), Y</t>
+  </si>
+  <si>
+    <t>Let 2004 = year 0, Year, X</t>
+  </si>
+  <si>
+    <t>Age (year), X</t>
+  </si>
+  <si>
+    <t>Cholesterol Level, Y</t>
+  </si>
+  <si>
+    <t>Let 31 = 0</t>
+  </si>
+  <si>
+    <t>Question 9</t>
   </si>
 </sst>
 </file>
@@ -8562,15 +8583,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725D82E5-2E75-4392-B55B-81B45DEC23B3}">
-  <dimension ref="A1:N106"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M104" sqref="M104"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L121" sqref="L121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10149,7 +10170,7 @@
         <v>500</v>
       </c>
       <c r="N94" s="1">
-        <f t="shared" ref="N93:N96" si="17">SUM(B94:M94)</f>
+        <f t="shared" ref="N94:N96" si="17">SUM(B94:M94)</f>
         <v>7449</v>
       </c>
     </row>
@@ -10616,6 +10637,433 @@
       <c r="K106" s="1">
         <f t="shared" si="21"/>
         <v>27418.6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+      <c r="E109">
+        <v>3</v>
+      </c>
+      <c r="F109">
+        <v>4</v>
+      </c>
+      <c r="G109">
+        <v>5</v>
+      </c>
+      <c r="H109">
+        <v>6</v>
+      </c>
+      <c r="I109" s="1">
+        <f>SUM(B109:H109)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B110">
+        <v>59</v>
+      </c>
+      <c r="C110">
+        <v>70</v>
+      </c>
+      <c r="D110">
+        <v>77</v>
+      </c>
+      <c r="E110">
+        <v>87</v>
+      </c>
+      <c r="F110">
+        <v>89</v>
+      </c>
+      <c r="G110">
+        <v>122</v>
+      </c>
+      <c r="H110">
+        <v>137</v>
+      </c>
+      <c r="I110" s="1">
+        <f>SUM(B110:H110)</f>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111">
+        <f>B109*B110</f>
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <f t="shared" ref="C111:H111" si="25">C109*C110</f>
+        <v>70</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="25"/>
+        <v>154</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="25"/>
+        <v>261</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="25"/>
+        <v>356</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="25"/>
+        <v>610</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="25"/>
+        <v>822</v>
+      </c>
+      <c r="I111" s="1">
+        <f>SUM(B111:H111)</f>
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112">
+        <f>B109^2</f>
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <f t="shared" ref="C112:H112" si="26">C109^2</f>
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="26"/>
+        <v>4</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="26"/>
+        <v>9</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="26"/>
+        <v>16</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="26"/>
+        <v>25</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="26"/>
+        <v>36</v>
+      </c>
+      <c r="I112" s="1">
+        <f>SUM(B112:H112)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113">
+        <f>B110^2</f>
+        <v>3481</v>
+      </c>
+      <c r="C113">
+        <f t="shared" ref="C113:H113" si="27">C110^2</f>
+        <v>4900</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="27"/>
+        <v>5929</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="27"/>
+        <v>7569</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="27"/>
+        <v>7921</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="27"/>
+        <v>14884</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="27"/>
+        <v>18769</v>
+      </c>
+      <c r="I113" s="1">
+        <f>SUM(B113:H113)</f>
+        <v>63453</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B117">
+        <f>31-31</f>
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <f>36-31</f>
+        <v>5</v>
+      </c>
+      <c r="D117">
+        <f>39-31</f>
+        <v>8</v>
+      </c>
+      <c r="E117">
+        <f>43-31</f>
+        <v>12</v>
+      </c>
+      <c r="F117">
+        <f>47-31</f>
+        <v>16</v>
+      </c>
+      <c r="G117">
+        <f>52-31</f>
+        <v>21</v>
+      </c>
+      <c r="H117">
+        <f>58-31</f>
+        <v>27</v>
+      </c>
+      <c r="I117">
+        <f>63-31</f>
+        <v>32</v>
+      </c>
+      <c r="J117">
+        <f>69-31</f>
+        <v>38</v>
+      </c>
+      <c r="K117">
+        <f>74-31</f>
+        <v>43</v>
+      </c>
+      <c r="L117" s="1">
+        <f>SUM(B117:K117)</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B118">
+        <v>165</v>
+      </c>
+      <c r="C118">
+        <v>181</v>
+      </c>
+      <c r="D118">
+        <v>177</v>
+      </c>
+      <c r="E118">
+        <v>193</v>
+      </c>
+      <c r="F118">
+        <v>213</v>
+      </c>
+      <c r="G118">
+        <v>191</v>
+      </c>
+      <c r="H118">
+        <v>189</v>
+      </c>
+      <c r="I118">
+        <v>154</v>
+      </c>
+      <c r="J118">
+        <v>235</v>
+      </c>
+      <c r="K118">
+        <v>198</v>
+      </c>
+      <c r="L118" s="1">
+        <f t="shared" ref="L118:L121" si="28">SUM(B118:K118)</f>
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119">
+        <f>B117*B118</f>
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <f t="shared" ref="C119:K119" si="29">C117*C118</f>
+        <v>905</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="29"/>
+        <v>1416</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="29"/>
+        <v>2316</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="29"/>
+        <v>3408</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="29"/>
+        <v>4011</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="29"/>
+        <v>5103</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="29"/>
+        <v>4928</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="29"/>
+        <v>8930</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="29"/>
+        <v>8514</v>
+      </c>
+      <c r="L119" s="1">
+        <f t="shared" si="28"/>
+        <v>39531</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <f>B117^2</f>
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ref="C120:K120" si="30">C117^2</f>
+        <v>25</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="30"/>
+        <v>64</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="30"/>
+        <v>144</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="30"/>
+        <v>256</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="30"/>
+        <v>441</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="30"/>
+        <v>729</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="30"/>
+        <v>1024</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="30"/>
+        <v>1444</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="30"/>
+        <v>1849</v>
+      </c>
+      <c r="L120" s="1">
+        <f t="shared" si="28"/>
+        <v>5976</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121">
+        <f>B118^2</f>
+        <v>27225</v>
+      </c>
+      <c r="C121">
+        <f t="shared" ref="C121:K121" si="31">C118^2</f>
+        <v>32761</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="31"/>
+        <v>31329</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="31"/>
+        <v>37249</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="31"/>
+        <v>45369</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="31"/>
+        <v>36481</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="31"/>
+        <v>35721</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="31"/>
+        <v>23716</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="31"/>
+        <v>55225</v>
+      </c>
+      <c r="K121">
+        <f t="shared" si="31"/>
+        <v>39204</v>
+      </c>
+      <c r="L121" s="1">
+        <f t="shared" si="28"/>
+        <v>364280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
y2s1: Week 13 Release 0.4
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/lectures/c8-tables.xlsx
+++ b/y2s1/statistics-ii/lectures/c8-tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC65F8BB-699D-4E23-A93F-CCB0DF351F89}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736323D8-F1A2-4B9F-BE11-E1FE997533E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1185" windowWidth="15375" windowHeight="7815" activeTab="1" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
+    <workbookView xWindow="6810" yWindow="930" windowWidth="15375" windowHeight="7815" activeTab="2" xr2:uid="{6A888A9F-4329-4A71-AAC2-210659982905}"/>
   </bookViews>
   <sheets>
     <sheet name="C8" sheetId="1" r:id="rId1"/>
     <sheet name="T8" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="109">
   <si>
     <t>X</t>
   </si>
@@ -261,6 +262,105 @@
   <si>
     <t>Question 9</t>
   </si>
+  <si>
+    <t>Spearman's rank correlation coefficient</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Spearman's Rank Correlation Coefficient</t>
+  </si>
+  <si>
+    <t>Sums</t>
+  </si>
+  <si>
+    <t>n^2-1</t>
+  </si>
+  <si>
+    <t>There is a moderate negative linear corelation between the weeks of experience and the number of rejects</t>
+  </si>
+  <si>
+    <t>W.O.E ( X )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.O.R. ( Y ) </t>
+  </si>
+  <si>
+    <t>b) PMCC</t>
+  </si>
+  <si>
+    <t>nEXY</t>
+  </si>
+  <si>
+    <t>EXEY</t>
+  </si>
+  <si>
+    <t>nEX^2-(EX)^2</t>
+  </si>
+  <si>
+    <t>nEY^2-(EY)^2</t>
+  </si>
+  <si>
+    <t>c)</t>
+  </si>
+  <si>
+    <t>SRCC</t>
+  </si>
+  <si>
+    <t>6Ed^2</t>
+  </si>
+  <si>
+    <t>4a</t>
+  </si>
+  <si>
+    <t>PMCC</t>
+  </si>
+  <si>
+    <t>Interp.</t>
+  </si>
+  <si>
+    <t>There is a high negative linear correlation between W.O.E. and N.O.R.</t>
+  </si>
+  <si>
+    <t>Interp</t>
+  </si>
+  <si>
+    <t>There is a high negative linear correlation between W.O.E. and N.O.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a high positive linear correlation between the total cost and the outputs of standard size boxes </t>
+  </si>
+  <si>
+    <t>4b</t>
+  </si>
+  <si>
+    <t>4c</t>
+  </si>
+  <si>
+    <t>X Rank</t>
+  </si>
+  <si>
+    <t>Y Rank</t>
+  </si>
+  <si>
+    <t>n(n^2-1)</t>
+  </si>
+  <si>
+    <t>6d^2</t>
+  </si>
+  <si>
+    <t>There is a very high positive linear correlation between the output and the cost of standard size boxes</t>
+  </si>
+  <si>
+    <t>d)</t>
+  </si>
+  <si>
+    <t>Estimate obtained in (b) is better than the estimate in ©, because C does not take in account of the impact of individual values and merely assigns a rank according to their size.</t>
+  </si>
 </sst>
 </file>
 
@@ -304,7 +404,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -613,11 +713,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -660,6 +769,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2487,6 +2617,781 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY"/>
+              <a:t>Employee</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N.O.R. ( Y ) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$I$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$44:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C417-487E-BAD9-A439F2641CA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="158438415"/>
+        <c:axId val="14425583"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="158438415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14425583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="14425583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="158438415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>total cost ($000) against output (’000 units) of standard size boxes </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-MY"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$89:$B$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$89:$C$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8BD-49FC-A05D-8A23B130B631}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1249007"/>
+        <c:axId val="1306175"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1249007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1306175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1306175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1249007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2647,6 +3552,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4182,6 +5167,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6362,6 +8379,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B24DBF9E-2753-419E-A50C-5D6FBDFA6014}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45618E52-3928-4CE0-9903-D56ABE11C226}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8585,8 +10679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725D82E5-2E75-4392-B55B-81B45DEC23B3}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L121" sqref="L121"/>
+    <sheetView topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11071,4 +13165,1884 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A503DFA-C3B5-44A9-AEC8-6A3188A1FF25}">
+  <dimension ref="A1:K162"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="D158" sqref="D158"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>7</v>
+      </c>
+      <c r="I4" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <f>B9-C9</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <f>D9^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ref="D10:D16" si="0">B10-C10</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10:E16" si="1">D10^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3">
+        <f>B12-C12</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <f>D12^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <f>SUM(E9:E16)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="40"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21">
+        <f>1-6*(E17)/(COUNTA(A9:A16)*(COUNTA(A9:A16)^2-1))</f>
+        <v>0.66666666666666674</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="3">
+        <v>4</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3">
+        <v>9</v>
+      </c>
+      <c r="I26" s="3">
+        <v>3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>10</v>
+      </c>
+      <c r="K26" s="43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>9</v>
+      </c>
+      <c r="H27" s="3">
+        <v>6</v>
+      </c>
+      <c r="I27" s="3">
+        <v>7</v>
+      </c>
+      <c r="J27" s="3">
+        <v>8</v>
+      </c>
+      <c r="K27" s="43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="3">
+        <f>B26-B27</f>
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" ref="C28:J28" si="2">C26-C27</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K28" s="43">
+        <f>K26-K27</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="3">
+        <f>B28^2</f>
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" ref="C29:J29" si="3">C28^2</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K29" s="43">
+        <f>K28^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34">
+        <f>SUM(B29:K29)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35">
+        <f>COUNTA(B25:K25)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36">
+        <f>B35^2-1</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37">
+        <f>1-6*B34/(B35*B36)</f>
+        <v>0.70909090909090911</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>9</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>12</v>
+      </c>
+      <c r="I43">
+        <v>14</v>
+      </c>
+      <c r="J43" s="1">
+        <f>SUM(B43:I43)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>22</v>
+      </c>
+      <c r="D44">
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <v>18</v>
+      </c>
+      <c r="F44">
+        <v>14</v>
+      </c>
+      <c r="G44">
+        <v>14</v>
+      </c>
+      <c r="H44">
+        <v>11</v>
+      </c>
+      <c r="I44">
+        <v>13</v>
+      </c>
+      <c r="J44" s="1">
+        <f>SUM(B44:I44)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <f>B43^2</f>
+        <v>16</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:I45" si="4">C43^2</f>
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="4"/>
+        <v>121</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="4"/>
+        <v>196</v>
+      </c>
+      <c r="J45">
+        <f>SUM(B45:I45)</f>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <f>B44^2</f>
+        <v>441</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:I46" si="5">C44^2</f>
+        <v>484</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="5"/>
+        <v>225</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="5"/>
+        <v>324</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="5"/>
+        <v>121</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="5"/>
+        <v>169</v>
+      </c>
+      <c r="J46">
+        <f>SUM(B46:I46)</f>
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <f>B43*B44</f>
+        <v>84</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:I47" si="6">C43*C44</f>
+        <v>110</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="6"/>
+        <v>105</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="6"/>
+        <v>162</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="6"/>
+        <v>140</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="6"/>
+        <v>154</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="6"/>
+        <v>132</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="6"/>
+        <v>182</v>
+      </c>
+      <c r="J47">
+        <f>SUM(B47:I47)</f>
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="F67" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="F68" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <f>J43</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <f>J44</f>
+        <v>128</v>
+      </c>
+      <c r="F70" t="s">
+        <v>51</v>
+      </c>
+      <c r="G70" t="s">
+        <v>83</v>
+      </c>
+      <c r="H70" t="s">
+        <v>84</v>
+      </c>
+      <c r="I70" t="s">
+        <v>58</v>
+      </c>
+      <c r="J70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="42">
+        <f>J47</f>
+        <v>1069</v>
+      </c>
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>7</v>
+      </c>
+      <c r="I71">
+        <f>G71-H71</f>
+        <v>-6</v>
+      </c>
+      <c r="J71">
+        <f>I71^2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="42">
+        <f>J45</f>
+        <v>732</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72">
+        <v>8</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72:I78" si="7">G72-H72</f>
+        <v>-6</v>
+      </c>
+      <c r="J72">
+        <f>I72^2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="42">
+        <f>J46</f>
+        <v>2156</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>5</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="J73">
+        <f t="shared" ref="J73:J78" si="8">I73^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74">
+        <f>COUNTA(B42:I42)</f>
+        <v>8</v>
+      </c>
+      <c r="F74" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74">
+        <v>4</v>
+      </c>
+      <c r="H74">
+        <v>6</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="F75" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75">
+        <v>5</v>
+      </c>
+      <c r="H75">
+        <v>3.5</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="8"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F76" t="s">
+        <v>15</v>
+      </c>
+      <c r="G76">
+        <v>6</v>
+      </c>
+      <c r="H76">
+        <v>3.5</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="8"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77">
+        <f>B74*B71</f>
+        <v>8552</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77">
+        <v>7</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78">
+        <f>B69*B70</f>
+        <v>9216</v>
+      </c>
+      <c r="F78" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78">
+        <v>8</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B79" s="42">
+        <f>B74*B72-(B69)^2</f>
+        <v>672</v>
+      </c>
+      <c r="J79" s="42">
+        <f>SUM(J71:J78)</f>
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B80" s="42">
+        <f>B74*B73-B70^2</f>
+        <v>864</v>
+      </c>
+      <c r="F80" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G80" s="42">
+        <f>J79*6</f>
+        <v>963</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F81" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="G81" s="42">
+        <f>COUNTA(F71:F78)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="42">
+        <f>(B77-B78)/SQRT(B79*B80)</f>
+        <v>-0.87141809054905162</v>
+      </c>
+      <c r="F82" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G82" s="42">
+        <f>G81^2-1</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="49"/>
+      <c r="D83" s="49"/>
+      <c r="E83" s="49"/>
+      <c r="F83" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G83" s="42">
+        <f>1-G80/(G81*G82)</f>
+        <v>-0.91071428571428581</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="49"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="49"/>
+      <c r="E84" s="49"/>
+      <c r="F84" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="G84" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="H84" s="49"/>
+      <c r="I84" s="49"/>
+      <c r="J84" s="49"/>
+    </row>
+    <row r="85" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G85" s="49"/>
+      <c r="H85" s="49"/>
+      <c r="I85" s="49"/>
+      <c r="J85" s="49"/>
+    </row>
+    <row r="86" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G86" s="50"/>
+      <c r="H86" s="50"/>
+      <c r="I86" s="50"/>
+      <c r="J86" s="50"/>
+    </row>
+    <row r="87" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89">
+        <v>20</v>
+      </c>
+      <c r="C89">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>4</v>
+      </c>
+      <c r="C91">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <v>23</v>
+      </c>
+      <c r="C92">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>18</v>
+      </c>
+      <c r="C93">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>6</v>
+      </c>
+      <c r="B94">
+        <v>14</v>
+      </c>
+      <c r="C94">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>7</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>8</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+      <c r="C96">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>9</v>
+      </c>
+      <c r="B97">
+        <v>13</v>
+      </c>
+      <c r="C97">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>10</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+      <c r="C98">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1</v>
+      </c>
+      <c r="B123">
+        <v>20</v>
+      </c>
+      <c r="C123">
+        <v>60</v>
+      </c>
+      <c r="D123">
+        <f>B123*C123</f>
+        <v>1200</v>
+      </c>
+      <c r="E123">
+        <f>B123^2</f>
+        <v>400</v>
+      </c>
+      <c r="F123">
+        <f>C123^2</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>2</v>
+      </c>
+      <c r="B124">
+        <v>2</v>
+      </c>
+      <c r="C124">
+        <v>25</v>
+      </c>
+      <c r="D124">
+        <f t="shared" ref="D124:D132" si="9">B124*C124</f>
+        <v>50</v>
+      </c>
+      <c r="E124">
+        <f t="shared" ref="E124:E132" si="10">B124^2</f>
+        <v>4</v>
+      </c>
+      <c r="F124">
+        <f t="shared" ref="F124:F132" si="11">C124^2</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>3</v>
+      </c>
+      <c r="B125">
+        <v>4</v>
+      </c>
+      <c r="C125">
+        <v>26</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="9"/>
+        <v>104</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="11"/>
+        <v>676</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>4</v>
+      </c>
+      <c r="B126">
+        <v>23</v>
+      </c>
+      <c r="C126">
+        <v>66</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="9"/>
+        <v>1518</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="10"/>
+        <v>529</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="11"/>
+        <v>4356</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>5</v>
+      </c>
+      <c r="B127">
+        <v>18</v>
+      </c>
+      <c r="C127">
+        <v>49</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="9"/>
+        <v>882</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="10"/>
+        <v>324</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="11"/>
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>6</v>
+      </c>
+      <c r="B128">
+        <v>14</v>
+      </c>
+      <c r="C128">
+        <v>48</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="9"/>
+        <v>672</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="10"/>
+        <v>196</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="11"/>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>7</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>35</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="9"/>
+        <v>350</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="11"/>
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>8</v>
+      </c>
+      <c r="B130">
+        <v>8</v>
+      </c>
+      <c r="C130">
+        <v>18</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="9"/>
+        <v>144</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="11"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>9</v>
+      </c>
+      <c r="B131">
+        <v>13</v>
+      </c>
+      <c r="C131">
+        <v>40</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="9"/>
+        <v>520</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="10"/>
+        <v>169</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="11"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>10</v>
+      </c>
+      <c r="B132">
+        <v>8</v>
+      </c>
+      <c r="C132">
+        <v>33</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="9"/>
+        <v>264</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="11"/>
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>31</v>
+      </c>
+      <c r="B133">
+        <f>SUM(B123:B132)</f>
+        <v>120</v>
+      </c>
+      <c r="C133">
+        <f>SUM(C123:C132)</f>
+        <v>400</v>
+      </c>
+      <c r="D133">
+        <f t="shared" ref="D133:F133" si="12">SUM(D123:D132)</f>
+        <v>5704</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="12"/>
+        <v>1866</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="12"/>
+        <v>18200</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>77</v>
+      </c>
+      <c r="B135">
+        <f>COUNTA(A123:A132)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>94</v>
+      </c>
+      <c r="B136">
+        <f>(B135*D133-B133*C133)/SQRT((B135*E133-(B133)^2)*(B135*F133-C133^2))</f>
+        <v>0.93379660473700177</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>95</v>
+      </c>
+      <c r="B137" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B139" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>1</v>
+      </c>
+      <c r="B142">
+        <v>9</v>
+      </c>
+      <c r="C142">
+        <v>9</v>
+      </c>
+      <c r="D142">
+        <f>B142-C142</f>
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <f>D142^2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>2</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <f t="shared" ref="D143:D151" si="13">B143-C143</f>
+        <v>-1</v>
+      </c>
+      <c r="E143">
+        <f t="shared" ref="E143:E151" si="14">D143^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>3</v>
+      </c>
+      <c r="B144">
+        <v>2</v>
+      </c>
+      <c r="C144">
+        <v>3</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>4</v>
+      </c>
+      <c r="B145">
+        <v>10</v>
+      </c>
+      <c r="C145">
+        <v>10</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>5</v>
+      </c>
+      <c r="B146">
+        <v>8</v>
+      </c>
+      <c r="C146">
+        <v>8</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>6</v>
+      </c>
+      <c r="B147">
+        <v>7</v>
+      </c>
+      <c r="C147">
+        <v>7</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>7</v>
+      </c>
+      <c r="B148">
+        <v>5</v>
+      </c>
+      <c r="C148">
+        <v>5</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>8</v>
+      </c>
+      <c r="B149">
+        <v>3.5</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="13"/>
+        <v>2.5</v>
+      </c>
+      <c r="E149">
+        <f t="shared" si="14"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>9</v>
+      </c>
+      <c r="B150">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <v>6</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>10</v>
+      </c>
+      <c r="B151">
+        <v>3.5</v>
+      </c>
+      <c r="C151">
+        <v>4</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="13"/>
+        <v>-0.5</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="14"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>5</v>
+      </c>
+      <c r="E152">
+        <f>SUM(E142:E151)</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>105</v>
+      </c>
+      <c r="B155">
+        <f>6*E152</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>104</v>
+      </c>
+      <c r="B156">
+        <f>COUNT(A142:A151)*(COUNT(A142:A151)^2-1)</f>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>91</v>
+      </c>
+      <c r="B157">
+        <f>1-B155/B156</f>
+        <v>0.94848484848484849</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>95</v>
+      </c>
+      <c r="B158" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>107</v>
+      </c>
+      <c r="B160" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B83:E84"/>
+    <mergeCell ref="G84:J85"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>